<commit_message>
ez lc upload fix
Former-commit-id: 09922d877f14158efc8884064c25f39edcf1cef6
</commit_message>
<xml_diff>
--- a/db/dummydata/ez_hubs.xlsx
+++ b/db/dummydata/ez_hubs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>STATUS</t>
   </si>
@@ -89,13 +89,37 @@
   </si>
   <si>
     <t>Waalhaven Zuidzijde 117, Rotterdam, Netherlands</t>
+  </si>
+  <si>
+    <t>Dalian</t>
+  </si>
+  <si>
+    <t>Yuejin Rd, Zhongshan Qu, Dalian Shi, Liaoning Sheng, China</t>
+  </si>
+  <si>
+    <t>Hong Kong, Kwun Tong, 偉業街223-231號,宏利金融中心B座7字樓,701A及708B室</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Sitra, Bahrain</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>Zhoushan, Zhejiang, China</t>
+  </si>
+  <si>
+    <t>https://assets.itsmycargo.com/assets/cityimages/Shanghai_sm.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -126,6 +150,14 @@
       <sz val="10.0"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -147,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -170,6 +202,21 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -369,29 +416,131 @@
       </c>
     </row>
     <row r="7" ht="12.0" customHeight="1">
-      <c r="F7" s="9"/>
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3">
+        <v>38.9310971</v>
+      </c>
+      <c r="F7" s="10">
+        <v>121.6590698</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" ht="12.0" customHeight="1">
-      <c r="F8" s="9"/>
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3">
+        <v>22.3081225</v>
+      </c>
+      <c r="F8" s="10">
+        <v>114.220595</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="9" ht="12.0" customHeight="1"/>
+    <row r="9" ht="12.0" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="3">
+        <v>26.1480232</v>
+      </c>
+      <c r="F9" s="10">
+        <v>50.6433176</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="10" ht="12.0" customHeight="1">
-      <c r="F10" s="9"/>
+      <c r="A10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="12">
+        <v>30.626539</v>
+      </c>
+      <c r="F10" s="12">
+        <v>122.064958</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="F11" s="9"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" ht="12.0" customHeight="1">
-      <c r="F12" s="9"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="F13" s="9"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
-      <c r="F14" s="9"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
-      <c r="F15" s="9"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" ht="12.0" customHeight="1"/>
     <row r="17" ht="12.0" customHeight="1"/>
@@ -1383,7 +1532,8 @@
     <hyperlink r:id="rId1" ref="I2"/>
     <hyperlink r:id="rId2" ref="I3"/>
     <hyperlink r:id="rId3" ref="I4"/>
+    <hyperlink r:id="rId4" ref="I10"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>